<commit_message>
Added row/column styles to E2E.
</commit_message>
<xml_diff>
--- a/test/e2e-generate/styles/out.xlsx
+++ b/test/e2e-generate/styles/out.xlsx
@@ -13,6 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -174,6 +177,9 @@
   </si>
   <si>
     <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foo</t>
   </si>
 </sst>
 </file>
@@ -271,6 +277,42 @@
     <font/>
     <font/>
     <font/>
+    <font>
+      <b/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+    </font>
+    <font>
+      <i/>
+    </font>
+    <font>
+      <i/>
+    </font>
+    <font>
+      <i/>
+      <b/>
+    </font>
+    <font>
+      <b/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+    </font>
+    <font>
+      <b/>
+    </font>
+    <font>
+      <b/>
+    </font>
+    <font>
+      <i/>
+    </font>
+    <font>
+      <i/>
+    </font>
   </fonts>
   <fills>
     <fill>
@@ -367,6 +409,17 @@
     <fill/>
     <fill/>
     <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
   </fills>
   <borders>
     <border>
@@ -689,6 +742,83 @@
       <diagonal style="thick">
         <color rgb="0000FF"/>
       </diagonal>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -842,6 +972,17 @@
     <xf fontId="48" fillId="49" borderId="48" applyFont="1" applyFill="1" applyBorder="1" numFmtId="12"/>
     <xf fontId="49" fillId="50" borderId="49" applyFont="1" applyFill="1" applyBorder="1" numFmtId="11"/>
     <xf fontId="50" fillId="51" borderId="50" applyFont="1" applyFill="1" applyBorder="1" numFmtId="49"/>
+    <xf fontId="51" fillId="52" borderId="51" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="52" fillId="53" borderId="52" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="53" fillId="54" borderId="53" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="54" fillId="55" borderId="54" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="55" fillId="56" borderId="55" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="56" fillId="57" borderId="56" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="57" fillId="58" borderId="57" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="58" fillId="59" borderId="58" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="59" fillId="60" borderId="59" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="60" fillId="61" borderId="60" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="61" fillId="62" borderId="61" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1415,4 +1556,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr/>
+  <cols>
+    <col min="1" max="1" style="51" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="53" customFormat="1">
+      <c r="A1" s="52"/>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr/>
+  <cols>
+    <col min="1" max="1" style="56" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="54" customFormat="1">
+      <c r="A1" t="s" s="55">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s" s="54">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="56">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr/>
+  <cols>
+    <col min="1" max="1" style="59" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="61" customFormat="1">
+      <c r="A1" t="s" s="57">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s" s="60">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="58">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>